<commit_message>
Slight tweak to stat card layout, spelling fixes
</commit_message>
<xml_diff>
--- a/stargravedata.xlsx
+++ b/stargravedata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Documents\Projects\Stargrave Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FEBC13-90B7-404F-BA92-6D1DC7FA03BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D2D215-418C-416C-B496-ADB289572C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11655" yWindow="-18405" windowWidth="34740" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13605" yWindow="-19740" windowWidth="27150" windowHeight="18675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -387,9 +387,6 @@
     <t>Repairbot</t>
   </si>
   <si>
-    <t>Robot, Unagressive</t>
-  </si>
-  <si>
     <t>Ruffian</t>
   </si>
   <si>
@@ -666,9 +663,6 @@
     <t>Animal, Amphibious, Immune to Toxin, Never Stunned</t>
   </si>
   <si>
-    <t>Large (-2F when shot at), Immune to Toxin, Terrifying Roar, Alpha Predator</t>
-  </si>
-  <si>
     <t>Large (-2F if shot at), Hatred of Gunfire, Immune to Radiation</t>
   </si>
   <si>
@@ -681,9 +675,6 @@
     <t>Heavy Armour, Knife, Hard to Target (+1F if shot at)</t>
   </si>
   <si>
-    <t>Light Armour, Knife, Hard to Target (+1F if shot at), Identify Weak Point (opponent gets -2A each combat rnd lost)</t>
-  </si>
-  <si>
     <t>Engineer</t>
   </si>
   <si>
@@ -720,9 +711,6 @@
     <t>Suffer equal damage when hits</t>
   </si>
   <si>
-    <t>Body of Energy, Limited Lifeforce, Levitate, Immune to Critical, Never Stunned/Wounded, Searing Touch (LP p81)</t>
-  </si>
-  <si>
     <t>Harvest Tick</t>
   </si>
   <si>
@@ -795,9 +783,6 @@
     <t>Comtech</t>
   </si>
   <si>
-    <t>Light Armour, Knife, Ship Systems Knowledge, +1 Unlock Data-Loot, Direct Comms (can activate out of range)</t>
-  </si>
-  <si>
     <t>Exosuit</t>
   </si>
   <si>
@@ -889,6 +874,21 @@
   </si>
   <si>
     <t>Blend in, Fire vulnerability, Master of Cover, Plant Biology</t>
+  </si>
+  <si>
+    <t>Large (-2F if shot at), Immune to Toxin, Terrifying Roar, Alpha Predator</t>
+  </si>
+  <si>
+    <t>Light Armour, Knife, Hard to Target (+1F if shot at), Identify Weak Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (LP p81)</t>
+  </si>
+  <si>
+    <t>Light Armour, Knife, Ship Systems Knowledge, +1 Unlock Data-Loot, Direct Comms</t>
+  </si>
+  <si>
+    <t>Robot, Unaggressive</t>
   </si>
 </sst>
 </file>
@@ -1252,14 +1252,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="M95" sqref="M95"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="10" width="8.7265625" style="2"/>
+    <col min="2" max="8" width="8.7265625" style="2"/>
+    <col min="9" max="9" width="98.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="2"/>
     <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -1304,7 +1306,7 @@
         <v>48</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1351,7 +1353,7 @@
         <v>-</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -1398,7 +1400,7 @@
         <v>-</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -1445,7 +1447,7 @@
         <v>-</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -1492,7 +1494,7 @@
         <v>-</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -1539,7 +1541,7 @@
         <v>-</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1586,7 +1588,7 @@
         <v>-</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -1633,7 +1635,7 @@
         <v>-</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1680,7 +1682,7 @@
         <v>-</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1727,7 +1729,7 @@
         <v>-</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1774,7 +1776,7 @@
         <v>-</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1821,7 +1823,7 @@
         <v>-</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1868,7 +1870,7 @@
         <v>-</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1915,7 +1917,7 @@
         <v>-</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1962,7 +1964,7 @@
         <v>-1 Shoot</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -2009,7 +2011,7 @@
         <v>-</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -2056,7 +2058,7 @@
         <v>2 targets</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -2103,7 +2105,7 @@
         <v>-</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -2150,7 +2152,7 @@
         <v>-</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -2197,7 +2199,7 @@
         <v>-</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -2226,7 +2228,7 @@
         <v>66</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>86</v>
@@ -2244,7 +2246,7 @@
         <v>-</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -2273,7 +2275,7 @@
         <v>66</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>54</v>
@@ -2291,7 +2293,7 @@
         <v>-</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
@@ -2338,7 +2340,7 @@
         <v>-</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
@@ -2385,7 +2387,7 @@
         <v>-</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -2414,7 +2416,7 @@
         <v>66</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>99</v>
@@ -2432,7 +2434,7 @@
         <v>+2 Fight if moved this act</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
@@ -2461,7 +2463,7 @@
         <v>66</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>102</v>
@@ -2479,7 +2481,7 @@
         <v>If Opp rolls F Nat 5-, take 2 Damage</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
@@ -2526,7 +2528,7 @@
         <v>-</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
@@ -2573,7 +2575,7 @@
         <v>-</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
@@ -2620,7 +2622,7 @@
         <v>-</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
@@ -2667,7 +2669,7 @@
         <v>-</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
@@ -2696,10 +2698,10 @@
         <v>66</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2714,7 +2716,7 @@
         <v>-</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
@@ -2743,7 +2745,7 @@
         <v>66</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>115</v>
+        <v>282</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>52</v>
@@ -2761,12 +2763,12 @@
         <v>-</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>20</v>
@@ -2805,12 +2807,12 @@
         <v>-</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>24</v>
@@ -2834,7 +2836,7 @@
         <v>66</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>60</v>
@@ -2852,12 +2854,12 @@
         <v>-</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>27</v>
@@ -2881,10 +2883,10 @@
         <v>66</v>
       </c>
       <c r="I35" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="K35" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2899,12 +2901,12 @@
         <v>Only triggered during enemy movement</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>27</v>
@@ -2928,10 +2930,10 @@
         <v>66</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K36" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2946,12 +2948,12 @@
         <v>-</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>20</v>
@@ -2975,10 +2977,10 @@
         <v>66</v>
       </c>
       <c r="I37" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="K37" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2993,12 +2995,12 @@
         <v>-</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>20</v>
@@ -3022,7 +3024,7 @@
         <v>66</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>60</v>
@@ -3040,12 +3042,12 @@
         <v>-</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>20</v>
@@ -3057,10 +3059,10 @@
         <v>41</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>21</v>
@@ -3069,7 +3071,7 @@
         <v>66</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>55</v>
@@ -3087,12 +3089,12 @@
         <v>-</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>24</v>
@@ -3107,19 +3109,19 @@
         <v>46</v>
       </c>
       <c r="F40" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I40" s="2" t="s">
+      <c r="J40" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="K40" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3134,12 +3136,12 @@
         <v>-</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>20</v>
@@ -3163,7 +3165,7 @@
         <v>66</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>60</v>
@@ -3181,12 +3183,12 @@
         <v>-</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>20</v>
@@ -3210,7 +3212,7 @@
         <v>66</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>99</v>
@@ -3228,12 +3230,12 @@
         <v>+2 Fight if moved this act</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>20</v>
@@ -3257,10 +3259,10 @@
         <v>66</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K43" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3275,12 +3277,12 @@
         <v>Never jams</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>20</v>
@@ -3304,7 +3306,7 @@
         <v>66</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>53</v>
@@ -3322,12 +3324,12 @@
         <v>-</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>20</v>
@@ -3351,7 +3353,7 @@
         <v>66</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>54</v>
@@ -3369,12 +3371,12 @@
         <v>-</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>20</v>
@@ -3398,7 +3400,7 @@
         <v>66</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>53</v>
@@ -3416,18 +3418,18 @@
         <v>-</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>12</v>
@@ -3436,19 +3438,19 @@
         <v>30</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>66</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>208</v>
+        <v>278</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K47" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3463,12 +3465,12 @@
         <v>-</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>20</v>
@@ -3492,10 +3494,10 @@
         <v>66</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K48" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3510,12 +3512,12 @@
         <v>-</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>20</v>
@@ -3527,7 +3529,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>41</v>
@@ -3539,7 +3541,7 @@
         <v>66</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>60</v>
@@ -3557,12 +3559,12 @@
         <v>-</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>85</v>
@@ -3586,10 +3588,10 @@
         <v>66</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K50" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3604,12 +3606,12 @@
         <v>-</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>20</v>
@@ -3633,7 +3635,7 @@
         <v>66</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>60</v>
@@ -3651,12 +3653,12 @@
         <v>-</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>20</v>
@@ -3680,7 +3682,7 @@
         <v>66</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>55</v>
@@ -3698,12 +3700,12 @@
         <v>-</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>20</v>
@@ -3730,7 +3732,7 @@
         <v>71</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K53" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3745,12 +3747,12 @@
         <v>Lose Damage bonus if jams</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>20</v>
@@ -3774,7 +3776,7 @@
         <v>31</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>54</v>
@@ -3792,12 +3794,12 @@
         <v>-</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>20</v>
@@ -3821,7 +3823,7 @@
         <v>31</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>52</v>
@@ -3839,12 +3841,12 @@
         <v>-</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>20</v>
@@ -3868,7 +3870,7 @@
         <v>14</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>54</v>
@@ -3886,12 +3888,12 @@
         <v>-</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>27</v>
@@ -3915,7 +3917,7 @@
         <v>31</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>55</v>
@@ -3933,12 +3935,12 @@
         <v>-</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>20</v>
@@ -3962,7 +3964,7 @@
         <v>34</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>55</v>
@@ -3980,12 +3982,12 @@
         <v>-</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>16</v>
@@ -4009,7 +4011,7 @@
         <v>66</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>86</v>
@@ -4027,12 +4029,12 @@
         <v>-</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>16</v>
@@ -4056,10 +4058,10 @@
         <v>66</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K60" s="1" t="str">
         <f t="shared" si="3"/>
@@ -4074,18 +4076,18 @@
         <v>-</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>12</v>
@@ -4094,7 +4096,7 @@
         <v>30</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>91</v>
@@ -4103,7 +4105,7 @@
         <v>66</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>60</v>
@@ -4121,12 +4123,12 @@
         <v>-</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>16</v>
@@ -4150,10 +4152,10 @@
         <v>66</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K62" s="1" t="str">
         <f t="shared" si="3"/>
@@ -4168,12 +4170,12 @@
         <v>-</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>16</v>
@@ -4197,10 +4199,10 @@
         <v>66</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K63" s="1" t="str">
         <f t="shared" si="3"/>
@@ -4215,12 +4217,12 @@
         <v>-</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>16</v>
@@ -4244,10 +4246,10 @@
         <v>66</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K64" s="1" t="str">
         <f t="shared" si="3"/>
@@ -4262,12 +4264,12 @@
         <v>-</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>27</v>
@@ -4291,7 +4293,7 @@
         <v>66</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>60</v>
@@ -4309,12 +4311,12 @@
         <v>-</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>27</v>
@@ -4338,13 +4340,13 @@
         <v>66</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>60</v>
       </c>
       <c r="K66" s="1" t="str">
-        <f t="shared" ref="K66:K97" si="6">VLOOKUP(J66,Weapons,2,FALSE)</f>
+        <f t="shared" ref="K66:K93" si="6">VLOOKUP(J66,Weapons,2,FALSE)</f>
         <v>-</v>
       </c>
       <c r="L66" s="1" t="str">
@@ -4356,12 +4358,12 @@
         <v>-</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>27</v>
@@ -4385,7 +4387,7 @@
         <v>66</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>55</v>
@@ -4403,18 +4405,18 @@
         <v>-</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>17</v>
@@ -4432,10 +4434,10 @@
         <v>34</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>213</v>
+        <v>279</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>17</v>
@@ -4444,15 +4446,15 @@
         <v>66</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>20</v>
@@ -4476,7 +4478,7 @@
         <v>14</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>53</v>
@@ -4494,12 +4496,12 @@
         <v>-</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>20</v>
@@ -4523,7 +4525,7 @@
         <v>34</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>55</v>
@@ -4541,12 +4543,12 @@
         <v>-</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>20</v>
@@ -4570,7 +4572,7 @@
         <v>34</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>55</v>
@@ -4588,18 +4590,18 @@
         <v>-</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>12</v>
@@ -4611,16 +4613,16 @@
         <v>28</v>
       </c>
       <c r="G72" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="J72" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K72" s="1">
         <f t="shared" si="6"/>
@@ -4635,12 +4637,12 @@
         <v>Will TN20 or Poisoned</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>20</v>
@@ -4655,7 +4657,7 @@
         <v>11</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>21</v>
@@ -4664,10 +4666,10 @@
         <v>66</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>226</v>
+        <v>280</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K73" s="1" t="str">
         <f t="shared" si="6"/>
@@ -4682,12 +4684,12 @@
         <v>Suffer equal damage when hits</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>85</v>
@@ -4711,7 +4713,7 @@
         <v>66</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>60</v>
@@ -4729,12 +4731,12 @@
         <v>-</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>20</v>
@@ -4758,7 +4760,7 @@
         <v>66</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>53</v>
@@ -4776,12 +4778,12 @@
         <v>-</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>20</v>
@@ -4805,7 +4807,7 @@
         <v>66</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>53</v>
@@ -4823,12 +4825,12 @@
         <v>-</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>27</v>
@@ -4852,10 +4854,10 @@
         <v>66</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="K77" s="1" t="str">
         <f t="shared" si="6"/>
@@ -4870,12 +4872,12 @@
         <v>-</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>20</v>
@@ -4899,7 +4901,7 @@
         <v>66</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>60</v>
@@ -4917,12 +4919,12 @@
         <v>-</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>24</v>
@@ -4946,10 +4948,10 @@
         <v>66</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K79" s="1" t="str">
         <f t="shared" si="6"/>
@@ -4964,12 +4966,12 @@
         <v>LP p86</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>14</v>
@@ -4993,10 +4995,10 @@
         <v>66</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="K80" s="1" t="str">
         <f t="shared" si="6"/>
@@ -5011,12 +5013,12 @@
         <v>Automatic attack, pull to combat if dmg</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>20</v>
@@ -5040,7 +5042,7 @@
         <v>21</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>55</v>
@@ -5058,12 +5060,12 @@
         <v>-</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>20</v>
@@ -5087,7 +5089,7 @@
         <v>34</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>55</v>
@@ -5105,12 +5107,12 @@
         <v>-</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>85</v>
@@ -5131,10 +5133,10 @@
         <v>30</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>55</v>
@@ -5152,12 +5154,12 @@
         <v>-</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>20</v>
@@ -5181,7 +5183,7 @@
         <v>34</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>55</v>
@@ -5199,12 +5201,12 @@
         <v>-</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>20</v>
@@ -5228,7 +5230,7 @@
         <v>34</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>54</v>
@@ -5246,12 +5248,12 @@
         <v>-</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>27</v>
@@ -5275,7 +5277,7 @@
         <v>66</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>55</v>
@@ -5293,39 +5295,39 @@
         <v>-</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>66</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K87" s="1" t="str">
         <f t="shared" si="6"/>
@@ -5340,12 +5342,12 @@
         <v>-</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>16</v>
@@ -5369,10 +5371,10 @@
         <v>66</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K88" s="1" t="str">
         <f t="shared" si="6"/>
@@ -5387,12 +5389,12 @@
         <v>Only triggered during enemy movement</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>27</v>
@@ -5416,10 +5418,10 @@
         <v>66</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>66</v>
@@ -5428,15 +5430,15 @@
         <v>66</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>20</v>
@@ -5451,7 +5453,7 @@
         <v>24</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>105</v>
@@ -5460,10 +5462,10 @@
         <v>66</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="K90" s="1" t="str">
         <f t="shared" si="6"/>
@@ -5478,12 +5480,12 @@
         <v>Use Will instead of S/F. No cover. Def A = 8+W</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>20</v>
@@ -5507,10 +5509,10 @@
         <v>66</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="K91" s="1" t="str">
         <f t="shared" si="6"/>
@@ -5525,18 +5527,18 @@
         <v>Treat as Flamethrower</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>12</v>
@@ -5554,10 +5556,10 @@
         <v>66</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K92" s="1" t="str">
         <f t="shared" si="6"/>
@@ -5572,12 +5574,12 @@
         <v>-</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>27</v>
@@ -5601,7 +5603,7 @@
         <v>66</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>112</v>
@@ -5619,7 +5621,7 @@
         <v>-</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -5850,7 +5852,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>66</v>
@@ -5859,12 +5861,12 @@
         <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>17</v>
@@ -5878,10 +5880,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>66</v>
@@ -5892,7 +5894,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>66</v>
@@ -5901,12 +5903,12 @@
         <v>70</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
@@ -5915,12 +5917,12 @@
         <v>70</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>10</v>
@@ -5934,7 +5936,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -5943,12 +5945,12 @@
         <v>64</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>66</v>
@@ -5957,12 +5959,12 @@
         <v>65</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>10</v>
@@ -5976,49 +5978,49 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>10</v>
@@ -6027,7 +6029,7 @@
         <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
"Assimilated" Death Vector enemies
</commit_message>
<xml_diff>
--- a/stargravedata.xlsx
+++ b/stargravedata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Documents\Projects\Stargrave Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benadmin/Library/CloudStorage/ProtonDrive-ben@kirman.org-folder/Projects/Game Aids and Accessories/Stargrave Cards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D2D215-418C-416C-B496-ADB289572C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5BC347-0C74-554B-A063-3961A9678149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13605" yWindow="-19740" windowWidth="27150" windowHeight="18675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="308">
   <si>
     <t>Name</t>
   </si>
@@ -889,6 +889,81 @@
   </si>
   <si>
     <t>Robot, Unaggressive</t>
+  </si>
+  <si>
+    <t>Acid Drake</t>
+  </si>
+  <si>
+    <t>Automaton</t>
+  </si>
+  <si>
+    <t>Automaton Bomb</t>
+  </si>
+  <si>
+    <t>Automaton Butcher</t>
+  </si>
+  <si>
+    <t>Automaton Hulk</t>
+  </si>
+  <si>
+    <t>Automaton Soldier</t>
+  </si>
+  <si>
+    <t>Automite</t>
+  </si>
+  <si>
+    <t>Cyberking</t>
+  </si>
+  <si>
+    <t>Cyberpawn</t>
+  </si>
+  <si>
+    <t>Cyrpent</t>
+  </si>
+  <si>
+    <t>Animal, Amphibious, Shooting Attack (6"), Toxic</t>
+  </si>
+  <si>
+    <t>Acid Spit</t>
+  </si>
+  <si>
+    <t>6"</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>Robot, Hatred of Gunfire, Pack Hunter (limit 4), Pistol, Dagger</t>
+  </si>
+  <si>
+    <t>Robot, Hatred of Gunfire, Pack Hunter (limit 4), Pistol, Dagger, Plasma Mine</t>
+  </si>
+  <si>
+    <t>Mine attack on 6. DV p72</t>
+  </si>
+  <si>
+    <t>Robot, Hatred of Gunfire, Pack Hunter (limit 4), Pistol, Dagger, Hand Weapon x 2, Sharp Teeth</t>
+  </si>
+  <si>
+    <t>Robot, Strong, Shotgun x 2, Hand Weapon</t>
+  </si>
+  <si>
+    <t>Two attacks</t>
+  </si>
+  <si>
+    <t>Robot, Carbine, Hand Weapon</t>
+  </si>
+  <si>
+    <t>Robot, Pack Hunter</t>
+  </si>
+  <si>
+    <t>(Movement defined by scenario)</t>
+  </si>
+  <si>
+    <t>Robot, Burrowing, Chamelon, Shooting Attack (6")</t>
+  </si>
+  <si>
+    <t>Shoot</t>
   </si>
 </sst>
 </file>
@@ -954,9 +1029,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -994,7 +1069,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1100,7 +1175,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1242,7 +1317,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1250,22 +1325,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N93"/>
+  <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="8" width="8.7265625" style="2"/>
-    <col min="9" max="9" width="98.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="2"/>
-    <col min="11" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="8" width="8.6640625" style="2"/>
+    <col min="9" max="9" width="98.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="2"/>
+    <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1384,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1356,7 +1431,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1403,7 +1478,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1450,7 +1525,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1497,7 +1572,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1544,7 +1619,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1591,7 +1666,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1638,7 +1713,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1685,7 +1760,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -1732,7 +1807,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -1779,7 +1854,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1826,7 +1901,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -1873,7 +1948,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1920,7 +1995,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1967,7 +2042,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -2014,7 +2089,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -2061,7 +2136,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -2108,7 +2183,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>84</v>
       </c>
@@ -2155,7 +2230,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>88</v>
       </c>
@@ -2202,7 +2277,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>90</v>
       </c>
@@ -2249,7 +2324,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>92</v>
       </c>
@@ -2296,7 +2371,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>93</v>
       </c>
@@ -2343,7 +2418,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>96</v>
       </c>
@@ -2390,7 +2465,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>98</v>
       </c>
@@ -2437,7 +2512,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>101</v>
       </c>
@@ -2484,7 +2559,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>104</v>
       </c>
@@ -2531,7 +2606,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>108</v>
       </c>
@@ -2578,7 +2653,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>109</v>
       </c>
@@ -2625,7 +2700,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>110</v>
       </c>
@@ -2672,7 +2747,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>113</v>
       </c>
@@ -2719,7 +2794,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>114</v>
       </c>
@@ -2766,7 +2841,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>115</v>
       </c>
@@ -2810,7 +2885,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>116</v>
       </c>
@@ -2857,7 +2932,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>118</v>
       </c>
@@ -2904,7 +2979,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
@@ -2951,7 +3026,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>125</v>
       </c>
@@ -2998,7 +3073,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>128</v>
       </c>
@@ -3045,7 +3120,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>130</v>
       </c>
@@ -3092,7 +3167,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>135</v>
       </c>
@@ -3139,7 +3214,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>140</v>
       </c>
@@ -3186,7 +3261,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>142</v>
       </c>
@@ -3233,7 +3308,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>143</v>
       </c>
@@ -3280,7 +3355,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>147</v>
       </c>
@@ -3327,7 +3402,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>149</v>
       </c>
@@ -3374,7 +3449,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>150</v>
       </c>
@@ -3421,7 +3496,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>152</v>
       </c>
@@ -3468,7 +3543,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>156</v>
       </c>
@@ -3515,7 +3590,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>158</v>
       </c>
@@ -3562,7 +3637,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>160</v>
       </c>
@@ -3609,7 +3684,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>161</v>
       </c>
@@ -3656,7 +3731,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>163</v>
       </c>
@@ -3703,7 +3778,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>165</v>
       </c>
@@ -3750,7 +3825,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>168</v>
       </c>
@@ -3797,7 +3872,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>170</v>
       </c>
@@ -3844,7 +3919,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>172</v>
       </c>
@@ -3891,7 +3966,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>174</v>
       </c>
@@ -3938,7 +4013,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>176</v>
       </c>
@@ -3985,7 +4060,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>178</v>
       </c>
@@ -4032,7 +4107,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>180</v>
       </c>
@@ -4079,7 +4154,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>182</v>
       </c>
@@ -4126,7 +4201,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>185</v>
       </c>
@@ -4173,7 +4248,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>186</v>
       </c>
@@ -4220,7 +4295,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>187</v>
       </c>
@@ -4267,7 +4342,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>189</v>
       </c>
@@ -4314,7 +4389,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>191</v>
       </c>
@@ -4361,7 +4436,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>193</v>
       </c>
@@ -4408,7 +4483,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>198</v>
       </c>
@@ -4452,7 +4527,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>202</v>
       </c>
@@ -4499,7 +4574,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>211</v>
       </c>
@@ -4546,7 +4621,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>213</v>
       </c>
@@ -4593,7 +4668,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>215</v>
       </c>
@@ -4640,7 +4715,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>220</v>
       </c>
@@ -4687,7 +4762,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>223</v>
       </c>
@@ -4734,7 +4809,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>225</v>
       </c>
@@ -4781,7 +4856,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>227</v>
       </c>
@@ -4828,7 +4903,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>228</v>
       </c>
@@ -4875,7 +4950,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>231</v>
       </c>
@@ -4922,7 +4997,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>233</v>
       </c>
@@ -4969,7 +5044,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>238</v>
       </c>
@@ -5016,7 +5091,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>243</v>
       </c>
@@ -5063,7 +5138,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>246</v>
       </c>
@@ -5110,7 +5185,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>247</v>
       </c>
@@ -5157,7 +5232,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>249</v>
       </c>
@@ -5204,7 +5279,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>251</v>
       </c>
@@ -5251,7 +5326,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>253</v>
       </c>
@@ -5298,7 +5373,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>256</v>
       </c>
@@ -5345,7 +5420,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>260</v>
       </c>
@@ -5392,7 +5467,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>262</v>
       </c>
@@ -5436,7 +5511,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>265</v>
       </c>
@@ -5483,7 +5558,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>270</v>
       </c>
@@ -5530,7 +5605,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>274</v>
       </c>
@@ -5577,7 +5652,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>276</v>
       </c>
@@ -5622,6 +5697,471 @@
       </c>
       <c r="N93" s="1" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="K94" s="1">
+        <f t="shared" ref="K94:K103" si="33">VLOOKUP(J94,Weapons,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="L94" s="1" t="str">
+        <f t="shared" ref="L94:L103" si="34">VLOOKUP(J94,Weapons,3,FALSE)</f>
+        <v>6"</v>
+      </c>
+      <c r="M94" s="1">
+        <f t="shared" ref="M94:M103" si="35">VLOOKUP(J94,Weapons,4,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N94" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K95" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="L95" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>10"</v>
+      </c>
+      <c r="M95" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="N95" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K96" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="L96" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>10"</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="N96" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K97" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>+1</v>
+      </c>
+      <c r="L97" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="M97" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="N97" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K98" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>+1</v>
+      </c>
+      <c r="L98" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>12"</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="N98" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K99" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="L99" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>24"</v>
+      </c>
+      <c r="M99" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K100" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="L100" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="M100" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="N100" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K101" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="L101" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="M101" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="N101" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K102" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="L102" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="M102" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="N102" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N103" s="1" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -5635,12 +6175,12 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -5654,7 +6194,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -5668,7 +6208,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -5682,7 +6222,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -5696,7 +6236,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -5710,7 +6250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -5724,7 +6264,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
@@ -5738,7 +6278,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>57</v>
       </c>
@@ -5752,7 +6292,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
@@ -5766,7 +6306,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
@@ -5780,7 +6320,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>60</v>
       </c>
@@ -5794,7 +6334,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -5808,7 +6348,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>99</v>
       </c>
@@ -5822,7 +6362,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
@@ -5836,7 +6376,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>112</v>
       </c>
@@ -5850,7 +6390,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>120</v>
       </c>
@@ -5864,7 +6404,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>127</v>
       </c>
@@ -5878,7 +6418,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>138</v>
       </c>
@@ -5892,7 +6432,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>144</v>
       </c>
@@ -5906,7 +6446,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>166</v>
       </c>
@@ -5920,7 +6460,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>203</v>
       </c>
@@ -5934,7 +6474,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>217</v>
       </c>
@@ -5948,7 +6488,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>221</v>
       </c>
@@ -5962,7 +6502,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>230</v>
       </c>
@@ -5976,7 +6516,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>235</v>
       </c>
@@ -5990,7 +6530,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>240</v>
       </c>
@@ -6004,7 +6544,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>267</v>
       </c>
@@ -6018,7 +6558,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>272</v>
       </c>
@@ -6032,115 +6572,119 @@
         <v>273</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>294</v>
+      </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>

</xml_diff>